<commit_message>
add new file analysis
</commit_message>
<xml_diff>
--- a/data/security.xlsx
+++ b/data/security.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tangbaonam/Documents/PROJECT/py_stkex/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B21B7F-9379-B344-B7CC-A28D1D5CD1D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="9540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="security" sheetId="4" r:id="rId1"/>
@@ -3493,7 +3499,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3551,6 +3557,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -3598,7 +3607,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3631,9 +3640,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3666,6 +3692,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3841,25 +3884,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H387"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="71.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="3" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="71.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="3"/>
+    <col min="9" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3885,7 +3928,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3908,7 +3951,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3931,7 +3974,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3954,7 +3997,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3977,7 +4020,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -4003,7 +4046,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -4026,7 +4069,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -4049,7 +4092,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -4072,7 +4115,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -4095,7 +4138,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -4118,7 +4161,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -4141,7 +4184,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -4164,7 +4207,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -4187,7 +4230,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -4210,7 +4253,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -4233,7 +4276,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -4256,7 +4299,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -4279,7 +4322,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -4302,7 +4345,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -4325,7 +4368,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -4348,7 +4391,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -4371,7 +4414,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -4394,7 +4437,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -4417,7 +4460,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -4440,7 +4483,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -4463,7 +4506,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -4486,7 +4529,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -4509,7 +4552,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -4532,7 +4575,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -4555,7 +4598,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -4578,7 +4621,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -4601,7 +4644,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -4624,7 +4667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -4647,7 +4690,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -4670,7 +4713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -4693,7 +4736,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -4716,7 +4759,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -4739,7 +4782,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -4762,7 +4805,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -4785,7 +4828,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -4808,7 +4851,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -4831,7 +4874,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -4854,7 +4897,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -4877,7 +4920,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -4900,7 +4943,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -4923,7 +4966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -4946,7 +4989,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -4969,7 +5012,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -4992,7 +5035,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -5015,7 +5058,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -5038,7 +5081,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -5061,7 +5104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -5084,7 +5127,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -5107,7 +5150,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -5130,7 +5173,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -5153,7 +5196,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -5176,7 +5219,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -5199,7 +5242,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -5222,7 +5265,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -5245,7 +5288,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -5268,7 +5311,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -5291,7 +5334,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -5314,7 +5357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -5337,7 +5380,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -5360,7 +5403,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -5383,7 +5426,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -5406,7 +5449,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -5429,7 +5472,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -5452,7 +5495,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -5475,7 +5518,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -5498,7 +5541,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -5521,7 +5564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -5544,7 +5587,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -5567,7 +5610,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -5590,7 +5633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -5613,7 +5656,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -5636,7 +5679,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -5659,7 +5702,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -5682,7 +5725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -5705,7 +5748,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -5728,7 +5771,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -5751,7 +5794,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -5774,7 +5817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -5797,7 +5840,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -5820,7 +5863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -5843,7 +5886,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -5866,7 +5909,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -5889,7 +5932,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -5912,7 +5955,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -5935,7 +5978,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -5958,7 +6001,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -5981,7 +6024,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -6004,7 +6047,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -6027,7 +6070,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -6050,7 +6093,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -6073,7 +6116,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -6096,7 +6139,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -6116,7 +6159,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -6139,7 +6182,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -6162,7 +6205,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -6185,7 +6228,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -6208,7 +6251,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -6231,7 +6274,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -6254,7 +6297,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -6277,7 +6320,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -6300,7 +6343,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -6323,7 +6366,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -6346,7 +6389,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -6369,7 +6412,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -6392,7 +6435,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -6415,7 +6458,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -6438,7 +6481,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -6461,7 +6504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -6481,7 +6524,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -6501,7 +6544,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A116" s="3">
         <v>115</v>
       </c>
@@ -6521,7 +6564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A117" s="3">
         <v>116</v>
       </c>
@@ -6541,7 +6584,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A118" s="3">
         <v>117</v>
       </c>
@@ -6561,7 +6604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A119" s="3">
         <v>118</v>
       </c>
@@ -6581,7 +6624,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A120" s="3">
         <v>119</v>
       </c>
@@ -6601,7 +6644,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A121" s="3">
         <v>120</v>
       </c>
@@ -6624,7 +6667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A122" s="3">
         <v>121</v>
       </c>
@@ -6647,7 +6690,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A123" s="3">
         <v>122</v>
       </c>
@@ -6670,7 +6713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A124" s="3">
         <v>123</v>
       </c>
@@ -6693,7 +6736,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A125" s="3">
         <v>124</v>
       </c>
@@ -6716,7 +6759,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A126" s="3">
         <v>125</v>
       </c>
@@ -6739,7 +6782,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A127" s="3">
         <v>126</v>
       </c>
@@ -6762,7 +6805,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A128" s="3">
         <v>127</v>
       </c>
@@ -6785,7 +6828,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A129" s="3">
         <v>128</v>
       </c>
@@ -6808,7 +6851,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A130" s="3">
         <v>129</v>
       </c>
@@ -6831,7 +6874,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A131" s="3">
         <v>130</v>
       </c>
@@ -6854,7 +6897,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A132" s="3">
         <v>131</v>
       </c>
@@ -6877,7 +6920,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A133" s="3">
         <v>132</v>
       </c>
@@ -6900,7 +6943,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A134" s="3">
         <v>133</v>
       </c>
@@ -6923,7 +6966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A135" s="3">
         <v>134</v>
       </c>
@@ -6946,7 +6989,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A136" s="3">
         <v>135</v>
       </c>
@@ -6969,7 +7012,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A137" s="3">
         <v>136</v>
       </c>
@@ -6992,7 +7035,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A138" s="3">
         <v>137</v>
       </c>
@@ -7015,7 +7058,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A139" s="3">
         <v>138</v>
       </c>
@@ -7038,7 +7081,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A140" s="3">
         <v>139</v>
       </c>
@@ -7061,7 +7104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A141" s="3">
         <v>140</v>
       </c>
@@ -7084,7 +7127,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A142" s="3">
         <v>141</v>
       </c>
@@ -7107,7 +7150,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A143" s="3">
         <v>142</v>
       </c>
@@ -7130,7 +7173,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A144" s="3">
         <v>143</v>
       </c>
@@ -7153,7 +7196,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A145" s="3">
         <v>144</v>
       </c>
@@ -7176,7 +7219,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A146" s="3">
         <v>145</v>
       </c>
@@ -7199,7 +7242,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A147" s="3">
         <v>146</v>
       </c>
@@ -7222,7 +7265,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A148" s="3">
         <v>147</v>
       </c>
@@ -7245,7 +7288,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A149" s="3">
         <v>148</v>
       </c>
@@ -7268,7 +7311,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A150" s="3">
         <v>149</v>
       </c>
@@ -7291,7 +7334,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A151" s="3">
         <v>150</v>
       </c>
@@ -7314,7 +7357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A152" s="3">
         <v>151</v>
       </c>
@@ -7337,7 +7380,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A153" s="3">
         <v>152</v>
       </c>
@@ -7360,7 +7403,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A154" s="3">
         <v>153</v>
       </c>
@@ -7383,7 +7426,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A155" s="3">
         <v>154</v>
       </c>
@@ -7406,7 +7449,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A156" s="3">
         <v>155</v>
       </c>
@@ -7429,7 +7472,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A157" s="3">
         <v>156</v>
       </c>
@@ -7452,7 +7495,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A158" s="3">
         <v>157</v>
       </c>
@@ -7475,7 +7518,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A159" s="3">
         <v>158</v>
       </c>
@@ -7498,7 +7541,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A160" s="3">
         <v>159</v>
       </c>
@@ -7521,7 +7564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A161" s="3">
         <v>160</v>
       </c>
@@ -7544,7 +7587,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A162" s="3">
         <v>161</v>
       </c>
@@ -7567,7 +7610,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A163" s="3">
         <v>162</v>
       </c>
@@ -7590,7 +7633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A164" s="3">
         <v>163</v>
       </c>
@@ -7613,7 +7656,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A165" s="3">
         <v>164</v>
       </c>
@@ -7636,7 +7679,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A166" s="3">
         <v>165</v>
       </c>
@@ -7659,7 +7702,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A167" s="3">
         <v>166</v>
       </c>
@@ -7682,7 +7725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A168" s="3">
         <v>167</v>
       </c>
@@ -7705,7 +7748,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A169" s="3">
         <v>168</v>
       </c>
@@ -7728,7 +7771,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A170" s="3">
         <v>169</v>
       </c>
@@ -7751,7 +7794,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A171" s="3">
         <v>170</v>
       </c>
@@ -7774,7 +7817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A172" s="3">
         <v>171</v>
       </c>
@@ -7797,7 +7840,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A173" s="3">
         <v>172</v>
       </c>
@@ -7820,7 +7863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A174" s="3">
         <v>173</v>
       </c>
@@ -7843,7 +7886,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A175" s="3">
         <v>174</v>
       </c>
@@ -7866,7 +7909,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A176" s="3">
         <v>175</v>
       </c>
@@ -7889,7 +7932,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A177" s="3">
         <v>176</v>
       </c>
@@ -7912,7 +7955,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A178" s="3">
         <v>177</v>
       </c>
@@ -7935,7 +7978,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A179" s="3">
         <v>178</v>
       </c>
@@ -7958,7 +8001,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A180" s="3">
         <v>179</v>
       </c>
@@ -7981,7 +8024,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A181" s="3">
         <v>180</v>
       </c>
@@ -8004,7 +8047,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A182" s="3">
         <v>181</v>
       </c>
@@ -8027,7 +8070,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A183" s="3">
         <v>182</v>
       </c>
@@ -8050,7 +8093,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A184" s="3">
         <v>183</v>
       </c>
@@ -8073,7 +8116,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A185" s="3">
         <v>184</v>
       </c>
@@ -8096,7 +8139,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A186" s="3">
         <v>185</v>
       </c>
@@ -8119,7 +8162,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A187" s="3">
         <v>186</v>
       </c>
@@ -8142,7 +8185,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A188" s="3">
         <v>187</v>
       </c>
@@ -8165,7 +8208,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A189" s="3">
         <v>188</v>
       </c>
@@ -8188,7 +8231,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A190" s="3">
         <v>189</v>
       </c>
@@ -8211,7 +8254,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A191" s="3">
         <v>190</v>
       </c>
@@ -8234,7 +8277,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A192" s="3">
         <v>191</v>
       </c>
@@ -8257,7 +8300,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A193" s="3">
         <v>192</v>
       </c>
@@ -8280,7 +8323,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A194" s="3">
         <v>193</v>
       </c>
@@ -8303,7 +8346,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A195" s="3">
         <v>194</v>
       </c>
@@ -8326,7 +8369,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A196" s="3">
         <v>195</v>
       </c>
@@ -8349,7 +8392,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A197" s="3">
         <v>196</v>
       </c>
@@ -8372,7 +8415,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A198" s="3">
         <v>197</v>
       </c>
@@ -8395,7 +8438,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A199" s="3">
         <v>198</v>
       </c>
@@ -8418,7 +8461,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A200" s="3">
         <v>199</v>
       </c>
@@ -8441,7 +8484,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A201" s="3">
         <v>200</v>
       </c>
@@ -8464,7 +8507,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A202" s="3">
         <v>201</v>
       </c>
@@ -8487,7 +8530,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A203" s="3">
         <v>202</v>
       </c>
@@ -8510,7 +8553,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A204" s="3">
         <v>203</v>
       </c>
@@ -8533,7 +8576,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A205" s="3">
         <v>204</v>
       </c>
@@ -8556,7 +8599,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A206" s="3">
         <v>205</v>
       </c>
@@ -8579,7 +8622,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A207" s="3">
         <v>206</v>
       </c>
@@ -8602,7 +8645,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A208" s="3">
         <v>207</v>
       </c>
@@ -8625,7 +8668,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A209" s="3">
         <v>208</v>
       </c>
@@ -8648,7 +8691,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A210" s="3">
         <v>209</v>
       </c>
@@ -8671,7 +8714,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A211" s="3">
         <v>210</v>
       </c>
@@ -8694,7 +8737,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A212" s="3">
         <v>211</v>
       </c>
@@ -8717,7 +8760,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A213" s="3">
         <v>212</v>
       </c>
@@ -8740,7 +8783,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A214" s="3">
         <v>213</v>
       </c>
@@ -8763,7 +8806,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A215" s="3">
         <v>214</v>
       </c>
@@ -8786,7 +8829,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A216" s="3">
         <v>215</v>
       </c>
@@ -8809,7 +8852,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A217" s="3">
         <v>216</v>
       </c>
@@ -8832,7 +8875,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A218" s="3">
         <v>217</v>
       </c>
@@ -8855,7 +8898,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A219" s="3">
         <v>218</v>
       </c>
@@ -8878,7 +8921,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A220" s="3">
         <v>219</v>
       </c>
@@ -8901,7 +8944,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A221" s="3">
         <v>220</v>
       </c>
@@ -8924,7 +8967,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A222" s="3">
         <v>221</v>
       </c>
@@ -8947,7 +8990,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A223" s="3">
         <v>222</v>
       </c>
@@ -8970,7 +9013,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A224" s="3">
         <v>223</v>
       </c>
@@ -8993,7 +9036,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A225" s="3">
         <v>224</v>
       </c>
@@ -9016,7 +9059,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A226" s="3">
         <v>225</v>
       </c>
@@ -9039,7 +9082,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A227" s="3">
         <v>226</v>
       </c>
@@ -9062,7 +9105,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A228" s="3">
         <v>227</v>
       </c>
@@ -9085,7 +9128,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A229" s="3">
         <v>228</v>
       </c>
@@ -9108,7 +9151,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A230" s="3">
         <v>229</v>
       </c>
@@ -9131,7 +9174,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A231" s="3">
         <v>230</v>
       </c>
@@ -9154,7 +9197,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A232" s="3">
         <v>231</v>
       </c>
@@ -9177,7 +9220,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A233" s="3">
         <v>232</v>
       </c>
@@ -9200,7 +9243,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A234" s="3">
         <v>233</v>
       </c>
@@ -9223,7 +9266,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A235" s="3">
         <v>234</v>
       </c>
@@ -9246,7 +9289,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A236" s="3">
         <v>235</v>
       </c>
@@ -9269,7 +9312,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A237" s="3">
         <v>236</v>
       </c>
@@ -9292,7 +9335,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A238" s="3">
         <v>237</v>
       </c>
@@ -9315,7 +9358,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A239" s="3">
         <v>238</v>
       </c>
@@ -9338,7 +9381,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A240" s="3">
         <v>239</v>
       </c>
@@ -9364,7 +9407,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A241" s="3">
         <v>240</v>
       </c>
@@ -9387,7 +9430,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A242" s="3">
         <v>241</v>
       </c>
@@ -9410,7 +9453,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A243" s="3">
         <v>242</v>
       </c>
@@ -9433,7 +9476,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A244" s="3">
         <v>243</v>
       </c>
@@ -9456,7 +9499,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A245" s="3">
         <v>244</v>
       </c>
@@ -9479,7 +9522,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A246" s="3">
         <v>245</v>
       </c>
@@ -9502,7 +9545,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A247" s="3">
         <v>246</v>
       </c>
@@ -9525,7 +9568,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A248" s="3">
         <v>247</v>
       </c>
@@ -9548,7 +9591,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A249" s="3">
         <v>248</v>
       </c>
@@ -9571,7 +9614,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A250" s="3">
         <v>249</v>
       </c>
@@ -9594,7 +9637,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A251" s="3">
         <v>250</v>
       </c>
@@ -9617,7 +9660,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A252" s="3">
         <v>251</v>
       </c>
@@ -9640,7 +9683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A253" s="3">
         <v>252</v>
       </c>
@@ -9663,7 +9706,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A254" s="3">
         <v>253</v>
       </c>
@@ -9686,7 +9729,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A255" s="3">
         <v>254</v>
       </c>
@@ -9709,7 +9752,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A256" s="3">
         <v>255</v>
       </c>
@@ -9732,7 +9775,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A257" s="3">
         <v>256</v>
       </c>
@@ -9755,7 +9798,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A258" s="3">
         <v>257</v>
       </c>
@@ -9778,7 +9821,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A259" s="3">
         <v>258</v>
       </c>
@@ -9801,7 +9844,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A260" s="3">
         <v>259</v>
       </c>
@@ -9824,7 +9867,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A261" s="3">
         <v>260</v>
       </c>
@@ -9847,7 +9890,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A262" s="3">
         <v>261</v>
       </c>
@@ -9870,7 +9913,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A263" s="3">
         <v>262</v>
       </c>
@@ -9893,7 +9936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A264" s="3">
         <v>263</v>
       </c>
@@ -9916,7 +9959,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A265" s="3">
         <v>264</v>
       </c>
@@ -9939,7 +9982,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A266" s="3">
         <v>265</v>
       </c>
@@ -9962,7 +10005,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A267" s="3">
         <v>266</v>
       </c>
@@ -9985,7 +10028,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A268" s="3">
         <v>267</v>
       </c>
@@ -10008,7 +10051,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A269" s="3">
         <v>268</v>
       </c>
@@ -10031,7 +10074,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A270" s="3">
         <v>269</v>
       </c>
@@ -10054,7 +10097,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A271" s="3">
         <v>270</v>
       </c>
@@ -10077,7 +10120,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A272" s="3">
         <v>271</v>
       </c>
@@ -10100,7 +10143,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A273" s="3">
         <v>272</v>
       </c>
@@ -10123,7 +10166,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A274" s="3">
         <v>273</v>
       </c>
@@ -10146,7 +10189,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A275" s="3">
         <v>274</v>
       </c>
@@ -10169,7 +10212,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A276" s="3">
         <v>275</v>
       </c>
@@ -10192,7 +10235,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A277" s="3">
         <v>276</v>
       </c>
@@ -10215,7 +10258,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A278" s="3">
         <v>277</v>
       </c>
@@ -10238,7 +10281,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A279" s="3">
         <v>278</v>
       </c>
@@ -10261,7 +10304,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A280" s="3">
         <v>279</v>
       </c>
@@ -10284,7 +10327,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A281" s="3">
         <v>280</v>
       </c>
@@ -10307,7 +10350,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A282" s="3">
         <v>281</v>
       </c>
@@ -10330,7 +10373,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A283" s="3">
         <v>282</v>
       </c>
@@ -10353,7 +10396,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A284" s="3">
         <v>283</v>
       </c>
@@ -10376,7 +10419,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A285" s="3">
         <v>284</v>
       </c>
@@ -10399,7 +10442,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A286" s="3">
         <v>285</v>
       </c>
@@ -10422,7 +10465,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A287" s="3">
         <v>286</v>
       </c>
@@ -10445,7 +10488,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A288" s="3">
         <v>287</v>
       </c>
@@ -10468,7 +10511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A289" s="3">
         <v>288</v>
       </c>
@@ -10491,7 +10534,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A290" s="3">
         <v>289</v>
       </c>
@@ -10514,7 +10557,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A291" s="3">
         <v>290</v>
       </c>
@@ -10537,7 +10580,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A292" s="3">
         <v>291</v>
       </c>
@@ -10560,7 +10603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A293" s="3">
         <v>292</v>
       </c>
@@ -10583,7 +10626,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A294" s="3">
         <v>293</v>
       </c>
@@ -10606,7 +10649,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A295" s="3">
         <v>294</v>
       </c>
@@ -10629,7 +10672,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A296" s="3">
         <v>295</v>
       </c>
@@ -10652,7 +10695,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A297" s="3">
         <v>296</v>
       </c>
@@ -10675,7 +10718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A298" s="3">
         <v>297</v>
       </c>
@@ -10698,7 +10741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A299" s="3">
         <v>298</v>
       </c>
@@ -10721,7 +10764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A300" s="3">
         <v>299</v>
       </c>
@@ -10744,7 +10787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A301" s="3">
         <v>300</v>
       </c>
@@ -10767,7 +10810,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A302" s="3">
         <v>301</v>
       </c>
@@ -10790,7 +10833,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A303" s="3">
         <v>302</v>
       </c>
@@ -10813,7 +10856,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A304" s="3">
         <v>303</v>
       </c>
@@ -10836,7 +10879,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A305" s="3">
         <v>304</v>
       </c>
@@ -10859,7 +10902,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A306" s="3">
         <v>305</v>
       </c>
@@ -10882,7 +10925,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A307" s="3">
         <v>306</v>
       </c>
@@ -10905,7 +10948,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A308" s="3">
         <v>307</v>
       </c>
@@ -10928,7 +10971,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A309" s="3">
         <v>308</v>
       </c>
@@ -10951,7 +10994,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A310" s="3">
         <v>309</v>
       </c>
@@ -10974,7 +11017,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A311" s="3">
         <v>310</v>
       </c>
@@ -10997,7 +11040,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A312" s="3">
         <v>311</v>
       </c>
@@ -11020,7 +11063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A313" s="3">
         <v>312</v>
       </c>
@@ -11043,7 +11086,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A314" s="3">
         <v>313</v>
       </c>
@@ -11066,7 +11109,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A315" s="3">
         <v>314</v>
       </c>
@@ -11089,7 +11132,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A316" s="3">
         <v>315</v>
       </c>
@@ -11112,7 +11155,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A317" s="3">
         <v>316</v>
       </c>
@@ -11135,7 +11178,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A318" s="3">
         <v>317</v>
       </c>
@@ -11158,7 +11201,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A319" s="3">
         <v>318</v>
       </c>
@@ -11181,7 +11224,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A320" s="3">
         <v>319</v>
       </c>
@@ -11204,7 +11247,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A321" s="3">
         <v>320</v>
       </c>
@@ -11227,7 +11270,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A322" s="3">
         <v>321</v>
       </c>
@@ -11250,7 +11293,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A323" s="3">
         <v>322</v>
       </c>
@@ -11273,7 +11316,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A324" s="3">
         <v>323</v>
       </c>
@@ -11296,7 +11339,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A325" s="3">
         <v>324</v>
       </c>
@@ -11319,7 +11362,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A326" s="3">
         <v>325</v>
       </c>
@@ -11342,7 +11385,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A327" s="3">
         <v>326</v>
       </c>
@@ -11365,7 +11408,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A328" s="3">
         <v>327</v>
       </c>
@@ -11388,7 +11431,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A329" s="3">
         <v>328</v>
       </c>
@@ -11411,7 +11454,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A330" s="3">
         <v>329</v>
       </c>
@@ -11434,7 +11477,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A331" s="3">
         <v>330</v>
       </c>
@@ -11457,7 +11500,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A332" s="3">
         <v>331</v>
       </c>
@@ -11480,7 +11523,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A333" s="3">
         <v>332</v>
       </c>
@@ -11503,7 +11546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A334" s="3">
         <v>333</v>
       </c>
@@ -11526,7 +11569,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A335" s="3">
         <v>334</v>
       </c>
@@ -11549,7 +11592,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A336" s="3">
         <v>335</v>
       </c>
@@ -11572,7 +11615,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A337" s="3">
         <v>336</v>
       </c>
@@ -11595,7 +11638,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A338" s="3">
         <v>337</v>
       </c>
@@ -11618,7 +11661,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A339" s="3">
         <v>338</v>
       </c>
@@ -11641,7 +11684,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A340" s="3">
         <v>339</v>
       </c>
@@ -11664,7 +11707,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A341" s="3">
         <v>340</v>
       </c>
@@ -11687,7 +11730,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A342" s="3">
         <v>341</v>
       </c>
@@ -11710,7 +11753,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A343" s="3">
         <v>342</v>
       </c>
@@ -11733,7 +11776,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A344" s="3">
         <v>343</v>
       </c>
@@ -11756,7 +11799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A345" s="3">
         <v>344</v>
       </c>
@@ -11779,7 +11822,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A346" s="3">
         <v>345</v>
       </c>
@@ -11802,7 +11845,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A347" s="3">
         <v>346</v>
       </c>
@@ -11825,7 +11868,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A348" s="3">
         <v>347</v>
       </c>
@@ -11848,7 +11891,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A349" s="3">
         <v>348</v>
       </c>
@@ -11871,7 +11914,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A350" s="3">
         <v>349</v>
       </c>
@@ -11894,7 +11937,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A351" s="3">
         <v>350</v>
       </c>
@@ -11917,7 +11960,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A352" s="3">
         <v>351</v>
       </c>
@@ -11940,7 +11983,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A353" s="3">
         <v>352</v>
       </c>
@@ -11963,7 +12006,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A354" s="3">
         <v>353</v>
       </c>
@@ -11986,7 +12029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A355" s="3">
         <v>354</v>
       </c>
@@ -12009,7 +12052,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A356" s="3">
         <v>355</v>
       </c>
@@ -12032,7 +12075,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A357" s="3">
         <v>356</v>
       </c>
@@ -12055,7 +12098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A358" s="3">
         <v>357</v>
       </c>
@@ -12078,7 +12121,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="359" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A359" s="3">
         <v>358</v>
       </c>
@@ -12101,7 +12144,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A360" s="3">
         <v>359</v>
       </c>
@@ -12124,7 +12167,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A361" s="3">
         <v>360</v>
       </c>
@@ -12147,7 +12190,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="362" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A362" s="3">
         <v>361</v>
       </c>
@@ -12170,7 +12213,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="363" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A363" s="3">
         <v>362</v>
       </c>
@@ -12193,7 +12236,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="364" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A364" s="3">
         <v>363</v>
       </c>
@@ -12216,7 +12259,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="365" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A365" s="3">
         <v>364</v>
       </c>
@@ -12239,7 +12282,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="366" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A366" s="3">
         <v>365</v>
       </c>
@@ -12262,7 +12305,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="367" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A367" s="3">
         <v>366</v>
       </c>
@@ -12285,7 +12328,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="368" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A368" s="3">
         <v>367</v>
       </c>
@@ -12308,7 +12351,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A369" s="3">
         <v>368</v>
       </c>
@@ -12331,7 +12374,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="370" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A370" s="3">
         <v>369</v>
       </c>
@@ -12354,7 +12397,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="371" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A371" s="3">
         <v>370</v>
       </c>
@@ -12377,7 +12420,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A372" s="3">
         <v>371</v>
       </c>
@@ -12400,7 +12443,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="373" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A373" s="3">
         <v>372</v>
       </c>
@@ -12423,7 +12466,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="374" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A374" s="3">
         <v>373</v>
       </c>
@@ -12446,7 +12489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="375" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A375" s="3">
         <v>374</v>
       </c>
@@ -12469,7 +12512,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="376" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A376" s="3">
         <v>375</v>
       </c>
@@ -12492,7 +12535,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="377" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A377" s="3">
         <v>376</v>
       </c>
@@ -12515,7 +12558,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A378" s="3">
         <v>377</v>
       </c>
@@ -12538,7 +12581,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="379" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A379" s="3">
         <v>378</v>
       </c>
@@ -12561,7 +12604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="380" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A380" s="3">
         <v>379</v>
       </c>
@@ -12584,7 +12627,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="381" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A381" s="3">
         <v>380</v>
       </c>
@@ -12607,7 +12650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="382" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A382" s="3">
         <v>381</v>
       </c>
@@ -12630,7 +12673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="383" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A383" s="3">
         <v>382</v>
       </c>
@@ -12653,7 +12696,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="384" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A384" s="3">
         <v>383</v>
       </c>
@@ -12676,7 +12719,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A385" s="3">
         <v>384</v>
       </c>
@@ -12699,7 +12742,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A386" s="3">
         <v>385</v>
       </c>
@@ -12722,7 +12765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A387" s="3">
         <v>386</v>
       </c>

</xml_diff>